<commit_message>
Rebalance for TUM 2.2 release
</commit_message>
<xml_diff>
--- a/TUM Enchanted/Data/s/Creatures Cost TUM Lite Enchanted Edition.xlsx
+++ b/TUM Enchanted/Data/s/Creatures Cost TUM Lite Enchanted Edition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1200,8 +1200,8 @@
         <v>47010</v>
       </c>
       <c r="J28" s="1">
-        <f>(130*28)+(230*20)+(330*16)+(450*8)+(890*6)+(1860*4)+(8200*2)</f>
-        <v>46300</v>
+        <f>(130*28)+(230*20)+(330*16)+(450*8)+(890*6)+(1860*4)+(8100*2)</f>
+        <v>46100</v>
       </c>
       <c r="K28" s="1">
         <f>(60*50)+(350*14)+(500*14)+(500*14)+(680*10)+(1800*4)+(5000*2)</f>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="L28">
         <f>C28+D28+E28+F28+G28+H28+I28+J28+K28</f>
-        <v>412301</v>
+        <v>412101</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>